<commit_message>
Update the AutowareConfig for the TA to add the filter for the point map
</commit_message>
<xml_diff>
--- a/AD-EYE/TA/AutowareConfig.xlsx
+++ b/AD-EYE/TA/AutowareConfig.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adeye\AD-EYE_Core\AD-EYE\Experiments\Base_Map\Simulation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adeye\AD-EYE_Core\AD-EYE\TA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64877862-C39C-4D00-A04F-B39E7C7EAB71}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20E24F13-2131-4888-BA00-451C2EB5C8E5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="994" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1002" uniqueCount="242">
   <si>
     <t>tf_x</t>
   </si>
@@ -1145,10 +1145,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G237"/>
+  <dimension ref="A1:G239"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A108" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G132" sqref="G132"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1223,49 +1223,49 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>22</v>
+      <c r="A4" s="10" t="s">
+        <v>21</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>235</v>
+        <v>208</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E4" s="5">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="F4" s="5">
         <v>10</v>
       </c>
       <c r="G4" s="5">
-        <v>-0.77</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>22</v>
+      <c r="A5" s="10" t="s">
+        <v>21</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>235</v>
+        <v>208</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>1</v>
+        <v>66</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E5" s="5">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="F5" s="5">
-        <v>10</v>
+        <v>300</v>
       </c>
       <c r="G5" s="5">
-        <v>0</v>
+        <v>200</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1276,7 +1276,7 @@
         <v>235</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>5</v>
@@ -1288,7 +1288,7 @@
         <v>10</v>
       </c>
       <c r="G6" s="5">
-        <v>1.07</v>
+        <v>-0.77</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1299,7 +1299,7 @@
         <v>235</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>229</v>
+        <v>1</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>5</v>
@@ -1322,7 +1322,7 @@
         <v>235</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>5</v>
@@ -1334,7 +1334,7 @@
         <v>10</v>
       </c>
       <c r="G8" s="5">
-        <v>0</v>
+        <v>1.07</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1345,7 +1345,7 @@
         <v>235</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>4</v>
+        <v>229</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>5</v>
@@ -1365,106 +1365,110 @@
         <v>22</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>221</v>
+        <v>235</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>222</v>
+        <v>3</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5" t="s">
-        <v>223</v>
+        <v>5</v>
+      </c>
+      <c r="E10" s="5">
+        <v>-10</v>
+      </c>
+      <c r="F10" s="5">
+        <v>10</v>
+      </c>
+      <c r="G10" s="5">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>208</v>
+      <c r="B11" s="3" t="s">
+        <v>235</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E11" s="5">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="F11" s="5">
         <v>10</v>
       </c>
       <c r="G11" s="5">
-        <v>0.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>208</v>
+      <c r="B12" s="3" t="s">
+        <v>221</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>66</v>
+        <v>222</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="5">
-        <v>0</v>
-      </c>
-      <c r="F12" s="5">
-        <v>300</v>
-      </c>
-      <c r="G12" s="5">
-        <v>200</v>
+        <v>19</v>
+      </c>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>209</v>
+      <c r="B13" s="2" t="s">
+        <v>208</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E13" s="5">
         <v>0</v>
       </c>
       <c r="F13" s="5">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G13" s="5">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>209</v>
+      <c r="B14" s="2" t="s">
+        <v>208</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>9</v>
+        <v>66</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="E14" s="5">
+        <v>0</v>
+      </c>
+      <c r="F14" s="5">
+        <v>300</v>
+      </c>
       <c r="G14" s="5">
-        <v>1</v>
+        <v>200</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1475,14 +1479,18 @@
         <v>209</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5" t="b">
+        <v>20</v>
+      </c>
+      <c r="E15" s="5">
+        <v>0</v>
+      </c>
+      <c r="F15" s="5">
+        <v>3</v>
+      </c>
+      <c r="G15" s="5">
         <v>0</v>
       </c>
     </row>
@@ -1494,15 +1502,15 @@
         <v>209</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>63</v>
+        <v>19</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
-      <c r="G16" s="5" t="b">
-        <v>0</v>
+      <c r="G16" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1513,7 +1521,7 @@
         <v>209</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>63</v>
@@ -1532,15 +1540,15 @@
         <v>209</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
-      <c r="G18" s="5" t="s">
-        <v>67</v>
+      <c r="G18" s="5" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1551,19 +1559,15 @@
         <v>209</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E19" s="5">
-        <v>1</v>
-      </c>
-      <c r="F19" s="5">
-        <v>1</v>
-      </c>
-      <c r="G19" s="5">
-        <v>1</v>
+        <v>63</v>
+      </c>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1574,7 +1578,7 @@
         <v>209</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>19</v>
@@ -1582,7 +1586,7 @@
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1593,14 +1597,18 @@
         <v>209</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5" t="b">
+        <v>20</v>
+      </c>
+      <c r="E21" s="5">
+        <v>1</v>
+      </c>
+      <c r="F21" s="5">
+        <v>1</v>
+      </c>
+      <c r="G21" s="5">
         <v>1</v>
       </c>
     </row>
@@ -1612,15 +1620,15 @@
         <v>209</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>63</v>
+        <v>19</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
-      <c r="G22" s="5" t="b">
-        <v>0</v>
+      <c r="G22" s="5" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1631,7 +1639,7 @@
         <v>209</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>63</v>
@@ -1639,52 +1647,44 @@
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>224</v>
+        <v>22</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>235</v>
+        <v>209</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E24" s="5">
-        <v>-10</v>
-      </c>
-      <c r="F24" s="5">
-        <v>10</v>
-      </c>
-      <c r="G24" s="11" t="s">
-        <v>225</v>
+        <v>63</v>
+      </c>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>224</v>
+        <v>22</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>235</v>
+        <v>209</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E25" s="5">
-        <v>-10</v>
-      </c>
-      <c r="F25" s="5">
-        <v>10</v>
-      </c>
-      <c r="G25" s="5">
+        <v>63</v>
+      </c>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1696,7 +1696,7 @@
         <v>235</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>5</v>
@@ -1707,8 +1707,8 @@
       <c r="F26" s="5">
         <v>10</v>
       </c>
-      <c r="G26" s="5" t="s">
-        <v>226</v>
+      <c r="G26" s="11" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1719,7 +1719,7 @@
         <v>235</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>229</v>
+        <v>1</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>5</v>
@@ -1742,7 +1742,7 @@
         <v>235</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>5</v>
@@ -1753,8 +1753,8 @@
       <c r="F28" s="5">
         <v>10</v>
       </c>
-      <c r="G28" s="5">
-        <v>0</v>
+      <c r="G28" s="5" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1765,7 +1765,7 @@
         <v>235</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>4</v>
+        <v>229</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>5</v>
@@ -1785,18 +1785,22 @@
         <v>224</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>221</v>
+        <v>235</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>222</v>
+        <v>3</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5" t="s">
-        <v>223</v>
+        <v>5</v>
+      </c>
+      <c r="E30" s="5">
+        <v>-10</v>
+      </c>
+      <c r="F30" s="5">
+        <v>10</v>
+      </c>
+      <c r="G30" s="5">
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1804,22 +1808,22 @@
         <v>224</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>208</v>
+        <v>235</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E31" s="5">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="F31" s="5">
         <v>10</v>
       </c>
-      <c r="G31" s="5" t="s">
-        <v>227</v>
+      <c r="G31" s="5">
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1827,68 +1831,64 @@
         <v>224</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>208</v>
+        <v>221</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>66</v>
+        <v>222</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E32" s="5">
-        <v>0</v>
-      </c>
-      <c r="F32" s="5">
-        <v>300</v>
-      </c>
-      <c r="G32" s="5">
-        <v>200</v>
+        <v>19</v>
+      </c>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>23</v>
+        <v>224</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>236</v>
+        <v>208</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E33" s="5">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="F33" s="5">
         <v>10</v>
       </c>
-      <c r="G33" s="5">
-        <v>0.31</v>
+      <c r="G33" s="5" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>23</v>
+        <v>224</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>236</v>
+        <v>208</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>1</v>
+        <v>66</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E34" s="5">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="F34" s="5">
-        <v>10</v>
+        <v>300</v>
       </c>
       <c r="G34" s="5">
-        <v>0</v>
+        <v>200</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -1899,7 +1899,7 @@
         <v>236</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>5</v>
@@ -1911,7 +1911,7 @@
         <v>10</v>
       </c>
       <c r="G35" s="5">
-        <v>0.63</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -1922,7 +1922,7 @@
         <v>236</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>69</v>
+        <v>1</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>5</v>
@@ -1934,7 +1934,7 @@
         <v>10</v>
       </c>
       <c r="G36" s="5">
-        <v>-0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -1945,7 +1945,7 @@
         <v>236</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>70</v>
+        <v>2</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>5</v>
@@ -1957,7 +1957,7 @@
         <v>10</v>
       </c>
       <c r="G37" s="5">
-        <v>0.5</v>
+        <v>0.63</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -1968,7 +1968,7 @@
         <v>236</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>5</v>
@@ -1991,7 +1991,7 @@
         <v>236</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>5</v>
@@ -2011,10 +2011,10 @@
         <v>23</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>0</v>
+        <v>71</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>5</v>
@@ -2026,7 +2026,7 @@
         <v>10</v>
       </c>
       <c r="G40" s="5">
-        <v>-0.49</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -2034,10 +2034,10 @@
         <v>23</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>1</v>
+        <v>72</v>
       </c>
       <c r="D41" s="5" t="s">
         <v>5</v>
@@ -2049,7 +2049,7 @@
         <v>10</v>
       </c>
       <c r="G41" s="5">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -2060,7 +2060,7 @@
         <v>237</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D42" s="5" t="s">
         <v>5</v>
@@ -2072,7 +2072,7 @@
         <v>10</v>
       </c>
       <c r="G42" s="5">
-        <v>1.1100000000000001</v>
+        <v>-0.49</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -2083,7 +2083,7 @@
         <v>237</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>69</v>
+        <v>1</v>
       </c>
       <c r="D43" s="5" t="s">
         <v>5</v>
@@ -2095,7 +2095,7 @@
         <v>10</v>
       </c>
       <c r="G43" s="5">
-        <v>-0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -2106,7 +2106,7 @@
         <v>237</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>70</v>
+        <v>2</v>
       </c>
       <c r="D44" s="5" t="s">
         <v>5</v>
@@ -2118,7 +2118,7 @@
         <v>10</v>
       </c>
       <c r="G44" s="5">
-        <v>0.5</v>
+        <v>1.1100000000000001</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -2129,7 +2129,7 @@
         <v>237</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D45" s="5" t="s">
         <v>5</v>
@@ -2152,7 +2152,7 @@
         <v>237</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D46" s="5" t="s">
         <v>5</v>
@@ -2171,38 +2171,46 @@
       <c r="A47" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B47" s="2" t="s">
-        <v>156</v>
+      <c r="B47" s="3" t="s">
+        <v>237</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>157</v>
+        <v>71</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E47" s="5"/>
-      <c r="F47" s="5"/>
-      <c r="G47" s="4" t="s">
-        <v>197</v>
+        <v>5</v>
+      </c>
+      <c r="E47" s="5">
+        <v>-10</v>
+      </c>
+      <c r="F47" s="5">
+        <v>10</v>
+      </c>
+      <c r="G47" s="5">
+        <v>-0.5</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B48" s="2" t="s">
-        <v>156</v>
+      <c r="B48" s="3" t="s">
+        <v>237</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>158</v>
+        <v>72</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E48" s="5"/>
-      <c r="F48" s="5"/>
-      <c r="G48" s="4" t="s">
-        <v>84</v>
+        <v>5</v>
+      </c>
+      <c r="E48" s="5">
+        <v>-10</v>
+      </c>
+      <c r="F48" s="5">
+        <v>10</v>
+      </c>
+      <c r="G48" s="5">
+        <v>0.5</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -2213,7 +2221,7 @@
         <v>156</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D49" s="5" t="s">
         <v>19</v>
@@ -2221,7 +2229,7 @@
       <c r="E49" s="5"/>
       <c r="F49" s="5"/>
       <c r="G49" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -2232,17 +2240,15 @@
         <v>156</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E50" s="5">
-        <v>0</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="E50" s="5"/>
       <c r="F50" s="5"/>
-      <c r="G50" s="4">
-        <v>720</v>
+      <c r="G50" s="4" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -2253,17 +2259,15 @@
         <v>156</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>50</v>
+        <v>159</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E51" s="5">
-        <v>0</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="E51" s="5"/>
       <c r="F51" s="5"/>
-      <c r="G51" s="4">
-        <v>960</v>
+      <c r="G51" s="4" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -2274,17 +2278,17 @@
         <v>156</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="E52" s="5">
         <v>0</v>
       </c>
       <c r="F52" s="5"/>
       <c r="G52" s="4">
-        <v>0</v>
+        <v>720</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -2295,17 +2299,17 @@
         <v>156</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>163</v>
+        <v>50</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="E53" s="5">
         <v>0</v>
       </c>
       <c r="F53" s="5"/>
       <c r="G53" s="4">
-        <v>0</v>
+        <v>960</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -2316,7 +2320,7 @@
         <v>156</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D54" s="5" t="s">
         <v>5</v>
@@ -2337,7 +2341,7 @@
         <v>156</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D55" s="5" t="s">
         <v>5</v>
@@ -2358,7 +2362,7 @@
         <v>156</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D56" s="5" t="s">
         <v>5</v>
@@ -2379,7 +2383,7 @@
         <v>156</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D57" s="5" t="s">
         <v>5</v>
@@ -2389,7 +2393,7 @@
       </c>
       <c r="F57" s="5"/>
       <c r="G57" s="4">
-        <v>1125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -2400,7 +2404,7 @@
         <v>156</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D58" s="5" t="s">
         <v>5</v>
@@ -2421,7 +2425,7 @@
         <v>156</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D59" s="5" t="s">
         <v>5</v>
@@ -2431,7 +2435,7 @@
       </c>
       <c r="F59" s="5"/>
       <c r="G59" s="4">
-        <v>480</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -2442,7 +2446,7 @@
         <v>156</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D60" s="5" t="s">
         <v>5</v>
@@ -2463,7 +2467,7 @@
         <v>156</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D61" s="5" t="s">
         <v>5</v>
@@ -2473,7 +2477,7 @@
       </c>
       <c r="F61" s="5"/>
       <c r="G61" s="4">
-        <v>1125</v>
+        <v>480</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -2484,7 +2488,7 @@
         <v>156</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D62" s="5" t="s">
         <v>5</v>
@@ -2494,7 +2498,7 @@
       </c>
       <c r="F62" s="5"/>
       <c r="G62" s="4">
-        <v>360</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -2505,7 +2509,7 @@
         <v>156</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D63" s="5" t="s">
         <v>5</v>
@@ -2515,7 +2519,7 @@
       </c>
       <c r="F63" s="5"/>
       <c r="G63" s="4">
-        <v>0</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -2526,7 +2530,7 @@
         <v>156</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D64" s="5" t="s">
         <v>5</v>
@@ -2536,7 +2540,7 @@
       </c>
       <c r="F64" s="5"/>
       <c r="G64" s="4">
-        <v>0</v>
+        <v>360</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -2547,7 +2551,7 @@
         <v>156</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D65" s="5" t="s">
         <v>5</v>
@@ -2557,7 +2561,7 @@
       </c>
       <c r="F65" s="5"/>
       <c r="G65" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -2568,7 +2572,7 @@
         <v>156</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D66" s="5" t="s">
         <v>5</v>
@@ -2578,7 +2582,7 @@
       </c>
       <c r="F66" s="5"/>
       <c r="G66" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -2589,7 +2593,7 @@
         <v>156</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D67" s="5" t="s">
         <v>5</v>
@@ -2599,7 +2603,7 @@
       </c>
       <c r="F67" s="5"/>
       <c r="G67" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
@@ -2610,7 +2614,7 @@
         <v>156</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D68" s="5" t="s">
         <v>5</v>
@@ -2620,7 +2624,7 @@
       </c>
       <c r="F68" s="5"/>
       <c r="G68" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -2631,7 +2635,7 @@
         <v>156</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D69" s="5" t="s">
         <v>5</v>
@@ -2652,7 +2656,7 @@
         <v>156</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D70" s="5" t="s">
         <v>5</v>
@@ -2662,7 +2666,7 @@
       </c>
       <c r="F70" s="5"/>
       <c r="G70" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
@@ -2673,7 +2677,7 @@
         <v>156</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D71" s="5" t="s">
         <v>5</v>
@@ -2694,7 +2698,7 @@
         <v>156</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D72" s="5" t="s">
         <v>5</v>
@@ -2704,7 +2708,7 @@
       </c>
       <c r="F72" s="5"/>
       <c r="G72" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -2715,7 +2719,7 @@
         <v>156</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D73" s="5" t="s">
         <v>5</v>
@@ -2736,7 +2740,7 @@
         <v>156</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D74" s="5" t="s">
         <v>5</v>
@@ -2746,7 +2750,7 @@
       </c>
       <c r="F74" s="5"/>
       <c r="G74" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -2757,7 +2761,7 @@
         <v>156</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D75" s="5" t="s">
         <v>5</v>
@@ -2767,7 +2771,7 @@
       </c>
       <c r="F75" s="5"/>
       <c r="G75" s="4">
-        <v>1125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
@@ -2778,7 +2782,7 @@
         <v>156</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D76" s="5" t="s">
         <v>5</v>
@@ -2788,7 +2792,7 @@
       </c>
       <c r="F76" s="5"/>
       <c r="G76" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -2799,7 +2803,7 @@
         <v>156</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D77" s="5" t="s">
         <v>5</v>
@@ -2809,7 +2813,7 @@
       </c>
       <c r="F77" s="5"/>
       <c r="G77" s="4">
-        <v>480</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
@@ -2820,7 +2824,7 @@
         <v>156</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D78" s="5" t="s">
         <v>5</v>
@@ -2841,7 +2845,7 @@
         <v>156</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D79" s="5" t="s">
         <v>5</v>
@@ -2851,7 +2855,7 @@
       </c>
       <c r="F79" s="5"/>
       <c r="G79" s="4">
-        <v>0</v>
+        <v>480</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
@@ -2862,7 +2866,7 @@
         <v>156</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D80" s="5" t="s">
         <v>5</v>
@@ -2872,7 +2876,7 @@
       </c>
       <c r="F80" s="5"/>
       <c r="G80" s="4">
-        <v>1125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
@@ -2883,7 +2887,7 @@
         <v>156</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D81" s="5" t="s">
         <v>5</v>
@@ -2893,7 +2897,7 @@
       </c>
       <c r="F81" s="5"/>
       <c r="G81" s="4">
-        <v>360</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
@@ -2904,7 +2908,7 @@
         <v>156</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D82" s="5" t="s">
         <v>5</v>
@@ -2914,7 +2918,7 @@
       </c>
       <c r="F82" s="5"/>
       <c r="G82" s="4">
-        <v>0</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -2925,7 +2929,7 @@
         <v>156</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D83" s="5" t="s">
         <v>5</v>
@@ -2935,7 +2939,7 @@
       </c>
       <c r="F83" s="5"/>
       <c r="G83" s="4">
-        <v>0</v>
+        <v>360</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
@@ -2946,7 +2950,7 @@
         <v>156</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D84" s="5" t="s">
         <v>5</v>
@@ -2967,7 +2971,7 @@
         <v>156</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D85" s="5" t="s">
         <v>5</v>
@@ -2977,7 +2981,7 @@
       </c>
       <c r="F85" s="5"/>
       <c r="G85" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -2988,7 +2992,7 @@
         <v>156</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D86" s="5" t="s">
         <v>5</v>
@@ -3006,18 +3010,20 @@
         <v>23</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>196</v>
+        <v>156</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>157</v>
+        <v>194</v>
       </c>
       <c r="D87" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E87" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="E87" s="5">
+        <v>0</v>
+      </c>
       <c r="F87" s="5"/>
-      <c r="G87" s="4" t="s">
-        <v>199</v>
+      <c r="G87" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -3025,18 +3031,20 @@
         <v>23</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>196</v>
+        <v>156</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>158</v>
+        <v>195</v>
       </c>
       <c r="D88" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E88" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="E88" s="5">
+        <v>0</v>
+      </c>
       <c r="F88" s="5"/>
-      <c r="G88" s="4" t="s">
-        <v>200</v>
+      <c r="G88" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
@@ -3047,7 +3055,7 @@
         <v>196</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D89" s="5" t="s">
         <v>19</v>
@@ -3055,7 +3063,7 @@
       <c r="E89" s="5"/>
       <c r="F89" s="5"/>
       <c r="G89" s="4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
@@ -3066,17 +3074,15 @@
         <v>196</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E90" s="5">
-        <v>0</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="E90" s="5"/>
       <c r="F90" s="5"/>
-      <c r="G90" s="4">
-        <v>720</v>
+      <c r="G90" s="4" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
@@ -3087,17 +3093,15 @@
         <v>196</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>50</v>
+        <v>159</v>
       </c>
       <c r="D91" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E91" s="5">
-        <v>0</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="E91" s="5"/>
       <c r="F91" s="5"/>
-      <c r="G91" s="4">
-        <v>960</v>
+      <c r="G91" s="4" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
@@ -3108,17 +3112,17 @@
         <v>196</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D92" s="5" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="E92" s="5">
         <v>0</v>
       </c>
       <c r="F92" s="5"/>
       <c r="G92" s="4">
-        <v>0</v>
+        <v>720</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
@@ -3129,17 +3133,17 @@
         <v>196</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>163</v>
+        <v>50</v>
       </c>
       <c r="D93" s="5" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="E93" s="5">
         <v>0</v>
       </c>
       <c r="F93" s="5"/>
       <c r="G93" s="4">
-        <v>0</v>
+        <v>960</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
@@ -3150,7 +3154,7 @@
         <v>196</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D94" s="5" t="s">
         <v>5</v>
@@ -3171,7 +3175,7 @@
         <v>196</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D95" s="5" t="s">
         <v>5</v>
@@ -3192,7 +3196,7 @@
         <v>196</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D96" s="5" t="s">
         <v>5</v>
@@ -3213,7 +3217,7 @@
         <v>196</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D97" s="5" t="s">
         <v>5</v>
@@ -3223,7 +3227,7 @@
       </c>
       <c r="F97" s="5"/>
       <c r="G97" s="4">
-        <v>1125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
@@ -3234,7 +3238,7 @@
         <v>196</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D98" s="5" t="s">
         <v>5</v>
@@ -3255,7 +3259,7 @@
         <v>196</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D99" s="5" t="s">
         <v>5</v>
@@ -3265,7 +3269,7 @@
       </c>
       <c r="F99" s="5"/>
       <c r="G99" s="4">
-        <v>480</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
@@ -3276,7 +3280,7 @@
         <v>196</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D100" s="5" t="s">
         <v>5</v>
@@ -3297,7 +3301,7 @@
         <v>196</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D101" s="5" t="s">
         <v>5</v>
@@ -3307,7 +3311,7 @@
       </c>
       <c r="F101" s="5"/>
       <c r="G101" s="4">
-        <v>1125</v>
+        <v>480</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
@@ -3318,7 +3322,7 @@
         <v>196</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D102" s="5" t="s">
         <v>5</v>
@@ -3328,7 +3332,7 @@
       </c>
       <c r="F102" s="5"/>
       <c r="G102" s="4">
-        <v>360</v>
+        <v>0</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
@@ -3339,7 +3343,7 @@
         <v>196</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D103" s="5" t="s">
         <v>5</v>
@@ -3349,7 +3353,7 @@
       </c>
       <c r="F103" s="5"/>
       <c r="G103" s="4">
-        <v>0</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
@@ -3360,7 +3364,7 @@
         <v>196</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D104" s="5" t="s">
         <v>5</v>
@@ -3370,7 +3374,7 @@
       </c>
       <c r="F104" s="5"/>
       <c r="G104" s="4">
-        <v>0</v>
+        <v>360</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
@@ -3381,7 +3385,7 @@
         <v>196</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D105" s="5" t="s">
         <v>5</v>
@@ -3391,7 +3395,7 @@
       </c>
       <c r="F105" s="5"/>
       <c r="G105" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
@@ -3402,7 +3406,7 @@
         <v>196</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D106" s="5" t="s">
         <v>5</v>
@@ -3412,7 +3416,7 @@
       </c>
       <c r="F106" s="5"/>
       <c r="G106" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
@@ -3423,7 +3427,7 @@
         <v>196</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D107" s="5" t="s">
         <v>5</v>
@@ -3433,7 +3437,7 @@
       </c>
       <c r="F107" s="5"/>
       <c r="G107" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
@@ -3444,7 +3448,7 @@
         <v>196</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D108" s="5" t="s">
         <v>5</v>
@@ -3454,7 +3458,7 @@
       </c>
       <c r="F108" s="5"/>
       <c r="G108" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
@@ -3465,7 +3469,7 @@
         <v>196</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D109" s="5" t="s">
         <v>5</v>
@@ -3486,7 +3490,7 @@
         <v>196</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D110" s="5" t="s">
         <v>5</v>
@@ -3496,7 +3500,7 @@
       </c>
       <c r="F110" s="5"/>
       <c r="G110" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
@@ -3507,7 +3511,7 @@
         <v>196</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D111" s="5" t="s">
         <v>5</v>
@@ -3528,7 +3532,7 @@
         <v>196</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D112" s="5" t="s">
         <v>5</v>
@@ -3538,7 +3542,7 @@
       </c>
       <c r="F112" s="5"/>
       <c r="G112" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
@@ -3549,7 +3553,7 @@
         <v>196</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D113" s="5" t="s">
         <v>5</v>
@@ -3570,7 +3574,7 @@
         <v>196</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D114" s="5" t="s">
         <v>5</v>
@@ -3580,7 +3584,7 @@
       </c>
       <c r="F114" s="5"/>
       <c r="G114" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
@@ -3591,7 +3595,7 @@
         <v>196</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D115" s="5" t="s">
         <v>5</v>
@@ -3601,7 +3605,7 @@
       </c>
       <c r="F115" s="5"/>
       <c r="G115" s="4">
-        <v>1125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
@@ -3612,7 +3616,7 @@
         <v>196</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D116" s="5" t="s">
         <v>5</v>
@@ -3622,7 +3626,7 @@
       </c>
       <c r="F116" s="5"/>
       <c r="G116" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
@@ -3633,7 +3637,7 @@
         <v>196</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D117" s="5" t="s">
         <v>5</v>
@@ -3643,7 +3647,7 @@
       </c>
       <c r="F117" s="5"/>
       <c r="G117" s="4">
-        <v>480</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
@@ -3654,7 +3658,7 @@
         <v>196</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D118" s="5" t="s">
         <v>5</v>
@@ -3675,7 +3679,7 @@
         <v>196</v>
       </c>
       <c r="C119" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D119" s="5" t="s">
         <v>5</v>
@@ -3685,7 +3689,7 @@
       </c>
       <c r="F119" s="5"/>
       <c r="G119" s="4">
-        <v>0</v>
+        <v>480</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
@@ -3696,7 +3700,7 @@
         <v>196</v>
       </c>
       <c r="C120" s="4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D120" s="5" t="s">
         <v>5</v>
@@ -3706,7 +3710,7 @@
       </c>
       <c r="F120" s="5"/>
       <c r="G120" s="4">
-        <v>1125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
@@ -3717,7 +3721,7 @@
         <v>196</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D121" s="5" t="s">
         <v>5</v>
@@ -3727,7 +3731,7 @@
       </c>
       <c r="F121" s="5"/>
       <c r="G121" s="4">
-        <v>360</v>
+        <v>0</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
@@ -3738,7 +3742,7 @@
         <v>196</v>
       </c>
       <c r="C122" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D122" s="5" t="s">
         <v>5</v>
@@ -3748,7 +3752,7 @@
       </c>
       <c r="F122" s="5"/>
       <c r="G122" s="4">
-        <v>0</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
@@ -3759,7 +3763,7 @@
         <v>196</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D123" s="5" t="s">
         <v>5</v>
@@ -3769,7 +3773,7 @@
       </c>
       <c r="F123" s="5"/>
       <c r="G123" s="4">
-        <v>0</v>
+        <v>360</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
@@ -3780,7 +3784,7 @@
         <v>196</v>
       </c>
       <c r="C124" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D124" s="5" t="s">
         <v>5</v>
@@ -3801,7 +3805,7 @@
         <v>196</v>
       </c>
       <c r="C125" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D125" s="5" t="s">
         <v>5</v>
@@ -3811,7 +3815,7 @@
       </c>
       <c r="F125" s="5"/>
       <c r="G125" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
@@ -3822,7 +3826,7 @@
         <v>196</v>
       </c>
       <c r="C126" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D126" s="5" t="s">
         <v>5</v>
@@ -3840,17 +3844,19 @@
         <v>23</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
       <c r="C127" s="4" t="s">
-        <v>73</v>
+        <v>194</v>
       </c>
       <c r="D127" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E127" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="E127" s="5">
+        <v>0</v>
+      </c>
       <c r="F127" s="5"/>
-      <c r="G127" s="5" t="b">
+      <c r="G127" s="4">
         <v>1</v>
       </c>
     </row>
@@ -3859,21 +3865,19 @@
         <v>23</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
       <c r="C128" s="4" t="s">
-        <v>74</v>
+        <v>195</v>
       </c>
       <c r="D128" s="5" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E128" s="5">
         <v>0</v>
       </c>
-      <c r="F128" s="5">
-        <v>3</v>
-      </c>
-      <c r="G128" s="5">
+      <c r="F128" s="5"/>
+      <c r="G128" s="4">
         <v>0</v>
       </c>
     </row>
@@ -3885,19 +3889,15 @@
         <v>210</v>
       </c>
       <c r="C129" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D129" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E129" s="5">
-        <v>0</v>
-      </c>
-      <c r="F129" s="5">
+        <v>63</v>
+      </c>
+      <c r="E129" s="5"/>
+      <c r="F129" s="5"/>
+      <c r="G129" s="5" t="b">
         <v>1</v>
-      </c>
-      <c r="G129" s="5">
-        <v>0.5</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
@@ -3908,15 +3908,19 @@
         <v>210</v>
       </c>
       <c r="C130" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D130" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E130" s="5"/>
-      <c r="F130" s="5"/>
-      <c r="G130" s="8" t="s">
-        <v>240</v>
+        <v>20</v>
+      </c>
+      <c r="E130" s="5">
+        <v>0</v>
+      </c>
+      <c r="F130" s="5">
+        <v>3</v>
+      </c>
+      <c r="G130" s="5">
+        <v>0</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
@@ -3927,15 +3931,19 @@
         <v>210</v>
       </c>
       <c r="C131" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D131" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E131" s="5"/>
-      <c r="F131" s="5"/>
-      <c r="G131" s="8" t="s">
-        <v>241</v>
+        <v>5</v>
+      </c>
+      <c r="E131" s="5">
+        <v>0</v>
+      </c>
+      <c r="F131" s="5">
+        <v>1</v>
+      </c>
+      <c r="G131" s="5">
+        <v>0.5</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
@@ -3946,7 +3954,7 @@
         <v>210</v>
       </c>
       <c r="C132" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D132" s="5" t="s">
         <v>19</v>
@@ -3954,7 +3962,7 @@
       <c r="E132" s="5"/>
       <c r="F132" s="5"/>
       <c r="G132" s="8" t="s">
-        <v>81</v>
+        <v>240</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
@@ -3965,7 +3973,7 @@
         <v>210</v>
       </c>
       <c r="C133" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D133" s="5" t="s">
         <v>19</v>
@@ -3973,7 +3981,7 @@
       <c r="E133" s="5"/>
       <c r="F133" s="5"/>
       <c r="G133" s="8" t="s">
-        <v>80</v>
+        <v>241</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
@@ -3981,10 +3989,10 @@
         <v>23</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>82</v>
+        <v>210</v>
       </c>
       <c r="C134" s="4" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D134" s="5" t="s">
         <v>19</v>
@@ -3992,7 +4000,7 @@
       <c r="E134" s="5"/>
       <c r="F134" s="5"/>
       <c r="G134" s="8" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
@@ -4000,10 +4008,10 @@
         <v>23</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>82</v>
+        <v>210</v>
       </c>
       <c r="C135" s="4" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D135" s="5" t="s">
         <v>19</v>
@@ -4011,7 +4019,7 @@
       <c r="E135" s="5"/>
       <c r="F135" s="5"/>
       <c r="G135" s="8" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
@@ -4022,19 +4030,15 @@
         <v>82</v>
       </c>
       <c r="C136" s="4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D136" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E136" s="5">
-        <v>-10</v>
-      </c>
-      <c r="F136" s="5">
-        <v>10</v>
-      </c>
-      <c r="G136" s="5">
-        <v>1.2</v>
+        <v>19</v>
+      </c>
+      <c r="E136" s="5"/>
+      <c r="F136" s="5"/>
+      <c r="G136" s="8" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
@@ -4042,18 +4046,18 @@
         <v>23</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C137" s="4" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D137" s="5" t="s">
         <v>19</v>
       </c>
       <c r="E137" s="5"/>
       <c r="F137" s="5"/>
-      <c r="G137" s="9" t="s">
-        <v>90</v>
+      <c r="G137" s="8" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
@@ -4061,18 +4065,22 @@
         <v>23</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C138" s="4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D138" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E138" s="5"/>
-      <c r="F138" s="5"/>
-      <c r="G138" s="5" t="b">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="E138" s="5">
+        <v>-10</v>
+      </c>
+      <c r="F138" s="5">
+        <v>10</v>
+      </c>
+      <c r="G138" s="5">
+        <v>1.2</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
@@ -4083,15 +4091,15 @@
         <v>88</v>
       </c>
       <c r="C139" s="4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D139" s="5" t="s">
-        <v>63</v>
+        <v>19</v>
       </c>
       <c r="E139" s="5"/>
       <c r="F139" s="5"/>
-      <c r="G139" s="5" t="b">
-        <v>0</v>
+      <c r="G139" s="9" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
@@ -4102,19 +4110,15 @@
         <v>88</v>
       </c>
       <c r="C140" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D140" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E140" s="5">
-        <v>0</v>
-      </c>
-      <c r="F140" s="5">
+        <v>63</v>
+      </c>
+      <c r="E140" s="5"/>
+      <c r="F140" s="5"/>
+      <c r="G140" s="5" t="b">
         <v>1</v>
-      </c>
-      <c r="G140" s="5">
-        <v>0.1</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
@@ -4125,17 +4129,15 @@
         <v>88</v>
       </c>
       <c r="C141" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D141" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E141" s="5">
-        <v>0</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="E141" s="5"/>
       <c r="F141" s="5"/>
-      <c r="G141" s="5">
-        <v>20</v>
+      <c r="G141" s="5" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.25">
@@ -4146,7 +4148,7 @@
         <v>88</v>
       </c>
       <c r="C142" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D142" s="5" t="s">
         <v>5</v>
@@ -4154,9 +4156,11 @@
       <c r="E142" s="5">
         <v>0</v>
       </c>
-      <c r="F142" s="5"/>
+      <c r="F142" s="5">
+        <v>1</v>
+      </c>
       <c r="G142" s="5">
-        <v>100000</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
@@ -4167,15 +4171,17 @@
         <v>88</v>
       </c>
       <c r="C143" s="4" t="s">
-        <v>18</v>
+        <v>94</v>
       </c>
       <c r="D143" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E143" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="E143" s="5">
+        <v>0</v>
+      </c>
       <c r="F143" s="5"/>
-      <c r="G143" s="5" t="b">
-        <v>0</v>
+      <c r="G143" s="5">
+        <v>20</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.25">
@@ -4186,15 +4192,17 @@
         <v>88</v>
       </c>
       <c r="C144" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D144" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E144" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="E144" s="5">
+        <v>0</v>
+      </c>
       <c r="F144" s="5"/>
-      <c r="G144" s="5" t="b">
-        <v>0</v>
+      <c r="G144" s="5">
+        <v>100000</v>
       </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.25">
@@ -4205,7 +4213,7 @@
         <v>88</v>
       </c>
       <c r="C145" s="4" t="s">
-        <v>97</v>
+        <v>18</v>
       </c>
       <c r="D145" s="5" t="s">
         <v>63</v>
@@ -4213,7 +4221,7 @@
       <c r="E145" s="5"/>
       <c r="F145" s="5"/>
       <c r="G145" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.25">
@@ -4224,19 +4232,15 @@
         <v>88</v>
       </c>
       <c r="C146" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D146" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E146" s="5">
-        <v>-10</v>
-      </c>
-      <c r="F146" s="5">
-        <v>10</v>
-      </c>
-      <c r="G146" s="5">
-        <v>-1.5</v>
+        <v>63</v>
+      </c>
+      <c r="E146" s="5"/>
+      <c r="F146" s="5"/>
+      <c r="G146" s="5" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.25">
@@ -4247,19 +4251,15 @@
         <v>88</v>
       </c>
       <c r="C147" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D147" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E147" s="5">
-        <v>-10</v>
-      </c>
-      <c r="F147" s="5">
-        <v>10</v>
-      </c>
-      <c r="G147" s="5">
-        <v>0.5</v>
+        <v>63</v>
+      </c>
+      <c r="E147" s="5"/>
+      <c r="F147" s="5"/>
+      <c r="G147" s="5" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
@@ -4270,15 +4270,19 @@
         <v>88</v>
       </c>
       <c r="C148" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D148" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E148" s="5"/>
-      <c r="F148" s="5"/>
-      <c r="G148" s="5" t="b">
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="E148" s="5">
+        <v>-10</v>
+      </c>
+      <c r="F148" s="5">
+        <v>10</v>
+      </c>
+      <c r="G148" s="5">
+        <v>-1.5</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.25">
@@ -4289,19 +4293,19 @@
         <v>88</v>
       </c>
       <c r="C149" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D149" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E149" s="5">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="F149" s="5">
         <v>10</v>
       </c>
       <c r="G149" s="5">
-        <v>5</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
@@ -4312,19 +4316,15 @@
         <v>88</v>
       </c>
       <c r="C150" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D150" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E150" s="5">
-        <v>0</v>
-      </c>
-      <c r="F150" s="5">
-        <v>11</v>
-      </c>
-      <c r="G150" s="5">
-        <v>5</v>
+        <v>63</v>
+      </c>
+      <c r="E150" s="5"/>
+      <c r="F150" s="5"/>
+      <c r="G150" s="5" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.25">
@@ -4335,7 +4335,7 @@
         <v>88</v>
       </c>
       <c r="C151" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D151" s="5" t="s">
         <v>5</v>
@@ -4344,10 +4344,10 @@
         <v>0</v>
       </c>
       <c r="F151" s="5">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="G151" s="5">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.25">
@@ -4358,7 +4358,7 @@
         <v>88</v>
       </c>
       <c r="C152" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D152" s="5" t="s">
         <v>5</v>
@@ -4367,10 +4367,10 @@
         <v>0</v>
       </c>
       <c r="F152" s="5">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G152" s="5">
-        <v>1.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
@@ -4381,7 +4381,7 @@
         <v>88</v>
       </c>
       <c r="C153" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D153" s="5" t="s">
         <v>5</v>
@@ -4390,10 +4390,10 @@
         <v>0</v>
       </c>
       <c r="F153" s="5">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G153" s="5">
-        <v>0.75</v>
+        <v>10</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.25">
@@ -4404,15 +4404,19 @@
         <v>88</v>
       </c>
       <c r="C154" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D154" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E154" s="5"/>
-      <c r="F154" s="5"/>
-      <c r="G154" s="5" t="b">
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="E154" s="5">
+        <v>0</v>
+      </c>
+      <c r="F154" s="5">
+        <v>10</v>
+      </c>
+      <c r="G154" s="5">
+        <v>1.5</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.25">
@@ -4423,15 +4427,19 @@
         <v>88</v>
       </c>
       <c r="C155" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D155" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E155" s="5"/>
-      <c r="F155" s="5"/>
-      <c r="G155" s="5" t="s">
-        <v>21</v>
+        <v>5</v>
+      </c>
+      <c r="E155" s="5">
+        <v>0</v>
+      </c>
+      <c r="F155" s="5">
+        <v>10</v>
+      </c>
+      <c r="G155" s="5">
+        <v>0.75</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.25">
@@ -4442,15 +4450,15 @@
         <v>88</v>
       </c>
       <c r="C156" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D156" s="5" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="E156" s="5"/>
       <c r="F156" s="5"/>
-      <c r="G156" s="5" t="s">
-        <v>114</v>
+      <c r="G156" s="5" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.25">
@@ -4461,7 +4469,7 @@
         <v>88</v>
       </c>
       <c r="C157" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D157" s="5" t="s">
         <v>19</v>
@@ -4469,7 +4477,7 @@
       <c r="E157" s="5"/>
       <c r="F157" s="5"/>
       <c r="G157" s="5" t="s">
-        <v>115</v>
+        <v>21</v>
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.25">
@@ -4480,15 +4488,15 @@
         <v>88</v>
       </c>
       <c r="C158" s="4" t="s">
-        <v>154</v>
+        <v>108</v>
       </c>
       <c r="D158" s="5" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="E158" s="5"/>
       <c r="F158" s="5"/>
-      <c r="G158" s="5">
-        <v>255</v>
+      <c r="G158" s="5" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.25">
@@ -4499,7 +4507,7 @@
         <v>88</v>
       </c>
       <c r="C159" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D159" s="5" t="s">
         <v>19</v>
@@ -4507,7 +4515,7 @@
       <c r="E159" s="5"/>
       <c r="F159" s="5"/>
       <c r="G159" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.25">
@@ -4518,19 +4526,15 @@
         <v>88</v>
       </c>
       <c r="C160" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D160" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E160" s="5">
-        <v>-10</v>
-      </c>
-      <c r="F160" s="5">
-        <v>10</v>
-      </c>
+      <c r="E160" s="5"/>
+      <c r="F160" s="5"/>
       <c r="G160" s="5">
-        <v>0</v>
+        <v>255</v>
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.25">
@@ -4541,15 +4545,15 @@
         <v>88</v>
       </c>
       <c r="C161" s="4" t="s">
-        <v>73</v>
+        <v>110</v>
       </c>
       <c r="D161" s="5" t="s">
-        <v>63</v>
+        <v>19</v>
       </c>
       <c r="E161" s="5"/>
       <c r="F161" s="5"/>
-      <c r="G161" s="5" t="b">
-        <v>0</v>
+      <c r="G161" s="5" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.25">
@@ -4560,14 +4564,18 @@
         <v>88</v>
       </c>
       <c r="C162" s="4" t="s">
-        <v>111</v>
+        <v>155</v>
       </c>
       <c r="D162" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E162" s="5"/>
-      <c r="F162" s="5"/>
-      <c r="G162" s="5" t="b">
+        <v>5</v>
+      </c>
+      <c r="E162" s="5">
+        <v>-10</v>
+      </c>
+      <c r="F162" s="5">
+        <v>10</v>
+      </c>
+      <c r="G162" s="5">
         <v>0</v>
       </c>
     </row>
@@ -4579,15 +4587,15 @@
         <v>88</v>
       </c>
       <c r="C163" s="4" t="s">
-        <v>112</v>
+        <v>73</v>
       </c>
       <c r="D163" s="5" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="E163" s="5"/>
       <c r="F163" s="5"/>
-      <c r="G163" s="5" t="s">
-        <v>117</v>
+      <c r="G163" s="5" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.25">
@@ -4598,15 +4606,15 @@
         <v>88</v>
       </c>
       <c r="C164" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D164" s="5" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="E164" s="5"/>
       <c r="F164" s="5"/>
-      <c r="G164" s="5" t="s">
-        <v>118</v>
+      <c r="G164" s="5" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.25">
@@ -4614,18 +4622,18 @@
         <v>23</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>119</v>
+        <v>88</v>
       </c>
       <c r="C165" s="4" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="D165" s="5" t="s">
         <v>19</v>
       </c>
       <c r="E165" s="5"/>
       <c r="F165" s="5"/>
-      <c r="G165" s="9" t="s">
-        <v>127</v>
+      <c r="G165" s="5" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.25">
@@ -4633,18 +4641,18 @@
         <v>23</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>119</v>
+        <v>88</v>
       </c>
       <c r="C166" s="4" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="D166" s="5" t="s">
         <v>19</v>
       </c>
       <c r="E166" s="5"/>
       <c r="F166" s="5"/>
-      <c r="G166" s="9" t="s">
-        <v>128</v>
+      <c r="G166" s="5" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.25">
@@ -4655,7 +4663,7 @@
         <v>119</v>
       </c>
       <c r="C167" s="4" t="s">
-        <v>83</v>
+        <v>120</v>
       </c>
       <c r="D167" s="5" t="s">
         <v>19</v>
@@ -4663,7 +4671,7 @@
       <c r="E167" s="5"/>
       <c r="F167" s="5"/>
       <c r="G167" s="9" t="s">
-        <v>84</v>
+        <v>127</v>
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.25">
@@ -4674,15 +4682,15 @@
         <v>119</v>
       </c>
       <c r="C168" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D168" s="5" t="s">
         <v>19</v>
       </c>
       <c r="E168" s="5"/>
       <c r="F168" s="5"/>
-      <c r="G168" s="5" t="s">
-        <v>129</v>
+      <c r="G168" s="9" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.25">
@@ -4693,15 +4701,15 @@
         <v>119</v>
       </c>
       <c r="C169" s="4" t="s">
-        <v>123</v>
+        <v>83</v>
       </c>
       <c r="D169" s="5" t="s">
         <v>19</v>
       </c>
       <c r="E169" s="5"/>
       <c r="F169" s="5"/>
-      <c r="G169" s="5" t="s">
-        <v>130</v>
+      <c r="G169" s="9" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.25">
@@ -4712,7 +4720,7 @@
         <v>119</v>
       </c>
       <c r="C170" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D170" s="5" t="s">
         <v>19</v>
@@ -4720,7 +4728,7 @@
       <c r="E170" s="5"/>
       <c r="F170" s="5"/>
       <c r="G170" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.25">
@@ -4731,15 +4739,15 @@
         <v>119</v>
       </c>
       <c r="C171" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D171" s="5" t="s">
-        <v>63</v>
+        <v>19</v>
       </c>
       <c r="E171" s="5"/>
       <c r="F171" s="5"/>
-      <c r="G171" s="5" t="b">
-        <v>0</v>
+      <c r="G171" s="5" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.25">
@@ -4750,19 +4758,15 @@
         <v>119</v>
       </c>
       <c r="C172" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D172" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E172" s="5">
-        <v>0</v>
-      </c>
-      <c r="F172" s="5">
-        <v>10</v>
-      </c>
-      <c r="G172" s="5">
-        <v>0.4</v>
+        <v>19</v>
+      </c>
+      <c r="E172" s="5"/>
+      <c r="F172" s="5"/>
+      <c r="G172" s="5" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.25">
@@ -4770,18 +4774,18 @@
         <v>23</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="C173" s="4" t="s">
-        <v>78</v>
+        <v>125</v>
       </c>
       <c r="D173" s="5" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="E173" s="5"/>
       <c r="F173" s="5"/>
-      <c r="G173" s="9" t="s">
-        <v>134</v>
+      <c r="G173" s="5" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.25">
@@ -4789,18 +4793,22 @@
         <v>23</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="C174" s="4" t="s">
-        <v>83</v>
+        <v>126</v>
       </c>
       <c r="D174" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E174" s="5"/>
-      <c r="F174" s="5"/>
-      <c r="G174" s="9" t="s">
-        <v>84</v>
+        <v>5</v>
+      </c>
+      <c r="E174" s="5">
+        <v>0</v>
+      </c>
+      <c r="F174" s="5">
+        <v>10</v>
+      </c>
+      <c r="G174" s="5">
+        <v>0.4</v>
       </c>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.25">
@@ -4811,15 +4819,15 @@
         <v>132</v>
       </c>
       <c r="C175" s="4" t="s">
-        <v>133</v>
+        <v>78</v>
       </c>
       <c r="D175" s="5" t="s">
-        <v>63</v>
+        <v>19</v>
       </c>
       <c r="E175" s="5"/>
       <c r="F175" s="5"/>
-      <c r="G175" s="5" t="b">
-        <v>0</v>
+      <c r="G175" s="9" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.25">
@@ -4827,10 +4835,10 @@
         <v>23</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C176" s="4" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="D176" s="5" t="s">
         <v>19</v>
@@ -4838,7 +4846,7 @@
       <c r="E176" s="5"/>
       <c r="F176" s="5"/>
       <c r="G176" s="9" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.25">
@@ -4846,18 +4854,18 @@
         <v>23</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C177" s="4" t="s">
-        <v>79</v>
+        <v>133</v>
       </c>
       <c r="D177" s="5" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="E177" s="5"/>
       <c r="F177" s="5"/>
-      <c r="G177" s="9" t="s">
-        <v>139</v>
+      <c r="G177" s="5" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.25">
@@ -4868,7 +4876,7 @@
         <v>135</v>
       </c>
       <c r="C178" s="4" t="s">
-        <v>136</v>
+        <v>78</v>
       </c>
       <c r="D178" s="5" t="s">
         <v>19</v>
@@ -4876,7 +4884,7 @@
       <c r="E178" s="5"/>
       <c r="F178" s="5"/>
       <c r="G178" s="9" t="s">
-        <v>140</v>
+        <v>81</v>
       </c>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.25">
@@ -4887,7 +4895,7 @@
         <v>135</v>
       </c>
       <c r="C179" s="4" t="s">
-        <v>137</v>
+        <v>79</v>
       </c>
       <c r="D179" s="5" t="s">
         <v>19</v>
@@ -4895,7 +4903,7 @@
       <c r="E179" s="5"/>
       <c r="F179" s="5"/>
       <c r="G179" s="9" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.25">
@@ -4906,7 +4914,7 @@
         <v>135</v>
       </c>
       <c r="C180" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D180" s="5" t="s">
         <v>19</v>
@@ -4914,49 +4922,45 @@
       <c r="E180" s="5"/>
       <c r="F180" s="5"/>
       <c r="G180" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
-        <v>213</v>
+        <v>23</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>212</v>
+        <v>135</v>
       </c>
       <c r="C181" s="4" t="s">
-        <v>24</v>
+        <v>137</v>
       </c>
       <c r="D181" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E181" s="5">
-        <v>0</v>
-      </c>
-      <c r="F181" s="5">
-        <v>2</v>
-      </c>
-      <c r="G181" s="5">
-        <v>0.75</v>
+        <v>19</v>
+      </c>
+      <c r="E181" s="5"/>
+      <c r="F181" s="5"/>
+      <c r="G181" s="9" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
-        <v>213</v>
+        <v>23</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>212</v>
+        <v>135</v>
       </c>
       <c r="C182" s="4" t="s">
-        <v>25</v>
+        <v>138</v>
       </c>
       <c r="D182" s="5" t="s">
-        <v>63</v>
+        <v>19</v>
       </c>
       <c r="E182" s="5"/>
       <c r="F182" s="5"/>
-      <c r="G182" s="5" t="b">
-        <v>1</v>
+      <c r="G182" s="9" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.25">
@@ -4967,15 +4971,19 @@
         <v>212</v>
       </c>
       <c r="C183" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D183" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E183" s="5"/>
-      <c r="F183" s="5"/>
-      <c r="G183" s="5" t="b">
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="E183" s="5">
+        <v>0</v>
+      </c>
+      <c r="F183" s="5">
+        <v>2</v>
+      </c>
+      <c r="G183" s="5">
+        <v>0.75</v>
       </c>
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.25">
@@ -4986,7 +4994,7 @@
         <v>212</v>
       </c>
       <c r="C184" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D184" s="5" t="s">
         <v>63</v>
@@ -5005,7 +5013,7 @@
         <v>212</v>
       </c>
       <c r="C185" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D185" s="5" t="s">
         <v>63</v>
@@ -5024,18 +5032,14 @@
         <v>212</v>
       </c>
       <c r="C186" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D186" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E186" s="5">
-        <v>0</v>
-      </c>
-      <c r="F186" s="5">
-        <v>2</v>
-      </c>
-      <c r="G186" s="5">
+        <v>63</v>
+      </c>
+      <c r="E186" s="5"/>
+      <c r="F186" s="5"/>
+      <c r="G186" s="5" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5047,18 +5051,14 @@
         <v>212</v>
       </c>
       <c r="C187" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D187" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E187" s="5">
-        <v>0</v>
-      </c>
-      <c r="F187" s="5">
-        <v>2</v>
-      </c>
-      <c r="G187" s="5">
+        <v>63</v>
+      </c>
+      <c r="E187" s="5"/>
+      <c r="F187" s="5"/>
+      <c r="G187" s="5" t="b">
         <v>0</v>
       </c>
     </row>
@@ -5070,15 +5070,19 @@
         <v>212</v>
       </c>
       <c r="C188" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D188" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E188" s="5"/>
-      <c r="F188" s="5"/>
-      <c r="G188" s="5" t="b">
-        <v>0</v>
+        <v>20</v>
+      </c>
+      <c r="E188" s="5">
+        <v>0</v>
+      </c>
+      <c r="F188" s="5">
+        <v>2</v>
+      </c>
+      <c r="G188" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.25">
@@ -5089,53 +5093,49 @@
         <v>212</v>
       </c>
       <c r="C189" s="4" t="s">
-        <v>239</v>
+        <v>30</v>
       </c>
       <c r="D189" s="5" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="E189" s="5">
         <v>0</v>
       </c>
       <c r="F189" s="5">
-        <v>100</v>
+        <v>2</v>
       </c>
       <c r="G189" s="5">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>65</v>
+        <v>212</v>
       </c>
       <c r="C190" s="4" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D190" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E190" s="5">
-        <v>0</v>
-      </c>
-      <c r="F190" s="5">
-        <v>10</v>
-      </c>
-      <c r="G190" s="5">
-        <v>0.75</v>
+        <v>63</v>
+      </c>
+      <c r="E190" s="5"/>
+      <c r="F190" s="5"/>
+      <c r="G190" s="5" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>65</v>
+        <v>212</v>
       </c>
       <c r="C191" s="4" t="s">
-        <v>32</v>
+        <v>239</v>
       </c>
       <c r="D191" s="5" t="s">
         <v>5</v>
@@ -5144,10 +5144,10 @@
         <v>0</v>
       </c>
       <c r="F191" s="5">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="G191" s="5">
-        <v>0.5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.25">
@@ -5158,7 +5158,7 @@
         <v>65</v>
       </c>
       <c r="C192" s="4" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="D192" s="5" t="s">
         <v>5</v>
@@ -5167,10 +5167,10 @@
         <v>0</v>
       </c>
       <c r="F192" s="5">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="G192" s="5">
-        <v>6</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.25">
@@ -5181,7 +5181,7 @@
         <v>65</v>
       </c>
       <c r="C193" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D193" s="5" t="s">
         <v>5</v>
@@ -5190,10 +5190,10 @@
         <v>0</v>
       </c>
       <c r="F193" s="5">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="G193" s="5">
-        <v>11.1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.25">
@@ -5204,7 +5204,7 @@
         <v>65</v>
       </c>
       <c r="C194" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D194" s="5" t="s">
         <v>5</v>
@@ -5213,10 +5213,10 @@
         <v>0</v>
       </c>
       <c r="F194" s="5">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="G194" s="5">
-        <v>0.1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.25">
@@ -5227,7 +5227,7 @@
         <v>65</v>
       </c>
       <c r="C195" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D195" s="5" t="s">
         <v>5</v>
@@ -5236,10 +5236,10 @@
         <v>0</v>
       </c>
       <c r="F195" s="5">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="G195" s="5">
-        <v>50</v>
+        <v>11.1</v>
       </c>
     </row>
     <row r="196" spans="1:7" x14ac:dyDescent="0.25">
@@ -5250,7 +5250,7 @@
         <v>65</v>
       </c>
       <c r="C196" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D196" s="5" t="s">
         <v>5</v>
@@ -5259,10 +5259,10 @@
         <v>0</v>
       </c>
       <c r="F196" s="5">
-        <v>500</v>
+        <v>50</v>
       </c>
       <c r="G196" s="5">
-        <v>200</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="197" spans="1:7" x14ac:dyDescent="0.25">
@@ -5273,7 +5273,7 @@
         <v>65</v>
       </c>
       <c r="C197" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D197" s="5" t="s">
         <v>5</v>
@@ -5282,10 +5282,10 @@
         <v>0</v>
       </c>
       <c r="F197" s="5">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="G197" s="5">
-        <v>20</v>
+        <v>50</v>
       </c>
     </row>
     <row r="198" spans="1:7" x14ac:dyDescent="0.25">
@@ -5296,7 +5296,7 @@
         <v>65</v>
       </c>
       <c r="C198" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D198" s="5" t="s">
         <v>5</v>
@@ -5305,10 +5305,10 @@
         <v>0</v>
       </c>
       <c r="F198" s="5">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="G198" s="5">
-        <v>15</v>
+        <v>200</v>
       </c>
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.25">
@@ -5319,7 +5319,7 @@
         <v>65</v>
       </c>
       <c r="C199" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D199" s="5" t="s">
         <v>5</v>
@@ -5331,7 +5331,7 @@
         <v>100</v>
       </c>
       <c r="G199" s="5">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.25">
@@ -5342,7 +5342,7 @@
         <v>65</v>
       </c>
       <c r="C200" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D200" s="5" t="s">
         <v>5</v>
@@ -5351,10 +5351,10 @@
         <v>0</v>
       </c>
       <c r="F200" s="5">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="G200" s="5">
-        <v>1.2</v>
+        <v>15</v>
       </c>
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.25">
@@ -5365,7 +5365,7 @@
         <v>65</v>
       </c>
       <c r="C201" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D201" s="5" t="s">
         <v>5</v>
@@ -5374,10 +5374,10 @@
         <v>0</v>
       </c>
       <c r="F201" s="5">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="G201" s="5">
-        <v>0.45</v>
+        <v>5</v>
       </c>
     </row>
     <row r="202" spans="1:7" x14ac:dyDescent="0.25">
@@ -5388,7 +5388,7 @@
         <v>65</v>
       </c>
       <c r="C202" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D202" s="5" t="s">
         <v>5</v>
@@ -5400,7 +5400,7 @@
         <v>10</v>
       </c>
       <c r="G202" s="5">
-        <v>0.4</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="203" spans="1:7" x14ac:dyDescent="0.25">
@@ -5411,7 +5411,7 @@
         <v>65</v>
       </c>
       <c r="C203" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D203" s="5" t="s">
         <v>5</v>
@@ -5423,7 +5423,7 @@
         <v>10</v>
       </c>
       <c r="G203" s="5">
-        <v>0.1</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="204" spans="1:7" x14ac:dyDescent="0.25">
@@ -5434,7 +5434,7 @@
         <v>65</v>
       </c>
       <c r="C204" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D204" s="5" t="s">
         <v>5</v>
@@ -5446,7 +5446,7 @@
         <v>10</v>
       </c>
       <c r="G204" s="5">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="205" spans="1:7" x14ac:dyDescent="0.25">
@@ -5457,15 +5457,19 @@
         <v>65</v>
       </c>
       <c r="C205" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D205" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E205" s="5"/>
-      <c r="F205" s="5"/>
-      <c r="G205" s="5" t="b">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="E205" s="5">
+        <v>0</v>
+      </c>
+      <c r="F205" s="5">
+        <v>10</v>
+      </c>
+      <c r="G205" s="5">
+        <v>0.1</v>
       </c>
     </row>
     <row r="206" spans="1:7" x14ac:dyDescent="0.25">
@@ -5476,15 +5480,19 @@
         <v>65</v>
       </c>
       <c r="C206" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D206" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E206" s="5"/>
-      <c r="F206" s="5"/>
-      <c r="G206" s="5" t="b">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="E206" s="5">
+        <v>0</v>
+      </c>
+      <c r="F206" s="5">
+        <v>10</v>
+      </c>
+      <c r="G206" s="5">
+        <v>0.1</v>
       </c>
     </row>
     <row r="207" spans="1:7" x14ac:dyDescent="0.25">
@@ -5495,7 +5503,7 @@
         <v>65</v>
       </c>
       <c r="C207" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D207" s="5" t="s">
         <v>63</v>
@@ -5514,7 +5522,7 @@
         <v>65</v>
       </c>
       <c r="C208" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D208" s="5" t="s">
         <v>63</v>
@@ -5522,7 +5530,7 @@
       <c r="E208" s="5"/>
       <c r="F208" s="5"/>
       <c r="G208" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="209" spans="1:7" x14ac:dyDescent="0.25">
@@ -5533,7 +5541,7 @@
         <v>65</v>
       </c>
       <c r="C209" s="4" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="D209" s="5" t="s">
         <v>63</v>
@@ -5552,19 +5560,15 @@
         <v>65</v>
       </c>
       <c r="C210" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D210" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E210" s="5">
-        <v>0</v>
-      </c>
-      <c r="F210" s="5">
-        <v>10</v>
-      </c>
-      <c r="G210" s="5">
-        <v>1.85</v>
+        <v>63</v>
+      </c>
+      <c r="E210" s="5"/>
+      <c r="F210" s="5"/>
+      <c r="G210" s="5" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="211" spans="1:7" x14ac:dyDescent="0.25">
@@ -5575,19 +5579,15 @@
         <v>65</v>
       </c>
       <c r="C211" s="4" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="D211" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E211" s="5">
-        <v>0</v>
-      </c>
-      <c r="F211" s="5">
-        <v>10</v>
-      </c>
-      <c r="G211" s="5">
-        <v>4.2</v>
+        <v>63</v>
+      </c>
+      <c r="E211" s="5"/>
+      <c r="F211" s="5"/>
+      <c r="G211" s="5" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="212" spans="1:7" x14ac:dyDescent="0.25">
@@ -5598,7 +5598,7 @@
         <v>65</v>
       </c>
       <c r="C212" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D212" s="5" t="s">
         <v>5</v>
@@ -5610,7 +5610,7 @@
         <v>10</v>
       </c>
       <c r="G212" s="5">
-        <v>2.7</v>
+        <v>1.85</v>
       </c>
     </row>
     <row r="213" spans="1:7" x14ac:dyDescent="0.25">
@@ -5621,7 +5621,7 @@
         <v>65</v>
       </c>
       <c r="C213" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D213" s="5" t="s">
         <v>5</v>
@@ -5633,7 +5633,7 @@
         <v>10</v>
       </c>
       <c r="G213" s="5">
-        <v>1</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="214" spans="1:7" x14ac:dyDescent="0.25">
@@ -5644,7 +5644,7 @@
         <v>65</v>
       </c>
       <c r="C214" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D214" s="5" t="s">
         <v>5</v>
@@ -5656,7 +5656,7 @@
         <v>10</v>
       </c>
       <c r="G214" s="5">
-        <v>0.8</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="215" spans="1:7" x14ac:dyDescent="0.25">
@@ -5667,7 +5667,7 @@
         <v>65</v>
       </c>
       <c r="C215" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D215" s="5" t="s">
         <v>5</v>
@@ -5679,7 +5679,7 @@
         <v>10</v>
       </c>
       <c r="G215" s="5">
-        <v>1.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="216" spans="1:7" x14ac:dyDescent="0.25">
@@ -5690,7 +5690,7 @@
         <v>65</v>
       </c>
       <c r="C216" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D216" s="5" t="s">
         <v>5</v>
@@ -5702,7 +5702,7 @@
         <v>10</v>
       </c>
       <c r="G216" s="5">
-        <v>3</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="217" spans="1:7" x14ac:dyDescent="0.25">
@@ -5713,7 +5713,7 @@
         <v>65</v>
       </c>
       <c r="C217" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D217" s="5" t="s">
         <v>5</v>
@@ -5725,7 +5725,7 @@
         <v>10</v>
       </c>
       <c r="G217" s="5">
-        <v>5</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="218" spans="1:7" x14ac:dyDescent="0.25">
@@ -5736,19 +5736,19 @@
         <v>65</v>
       </c>
       <c r="C218" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D218" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E218" s="5">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="F218" s="5">
         <v>10</v>
       </c>
       <c r="G218" s="5">
-        <v>-4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="219" spans="1:7" x14ac:dyDescent="0.25">
@@ -5759,7 +5759,7 @@
         <v>65</v>
       </c>
       <c r="C219" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D219" s="5" t="s">
         <v>5</v>
@@ -5771,7 +5771,7 @@
         <v>10</v>
       </c>
       <c r="G219" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="220" spans="1:7" x14ac:dyDescent="0.25">
@@ -5782,7 +5782,7 @@
         <v>65</v>
       </c>
       <c r="C220" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D220" s="5" t="s">
         <v>5</v>
@@ -5791,10 +5791,10 @@
         <v>-10</v>
       </c>
       <c r="F220" s="5">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G220" s="5">
-        <v>-3</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="221" spans="1:7" x14ac:dyDescent="0.25">
@@ -5805,19 +5805,19 @@
         <v>65</v>
       </c>
       <c r="C221" s="4" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="D221" s="5" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E221" s="5">
         <v>0</v>
       </c>
       <c r="F221" s="5">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="G221" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="222" spans="1:7" x14ac:dyDescent="0.25">
@@ -5825,18 +5825,22 @@
         <v>214</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C222" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D222" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E222" s="5"/>
-      <c r="F222" s="5"/>
-      <c r="G222" s="5" t="b">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="E222" s="5">
+        <v>-10</v>
+      </c>
+      <c r="F222" s="5">
+        <v>0</v>
+      </c>
+      <c r="G222" s="5">
+        <v>-3</v>
       </c>
     </row>
     <row r="223" spans="1:7" x14ac:dyDescent="0.25">
@@ -5844,17 +5848,21 @@
         <v>214</v>
       </c>
       <c r="B223" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C223" s="4" t="s">
-        <v>62</v>
+        <v>29</v>
       </c>
       <c r="D223" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E223" s="5"/>
-      <c r="F223" s="5"/>
-      <c r="G223" s="5" t="b">
+        <v>20</v>
+      </c>
+      <c r="E223" s="5">
+        <v>0</v>
+      </c>
+      <c r="F223" s="5">
+        <v>2</v>
+      </c>
+      <c r="G223" s="5">
         <v>1</v>
       </c>
     </row>
@@ -5863,10 +5871,10 @@
         <v>214</v>
       </c>
       <c r="B224" s="2" t="s">
-        <v>143</v>
+        <v>64</v>
       </c>
       <c r="C224" s="4" t="s">
-        <v>144</v>
+        <v>61</v>
       </c>
       <c r="D224" s="5" t="s">
         <v>63</v>
@@ -5882,22 +5890,18 @@
         <v>214</v>
       </c>
       <c r="B225" s="2" t="s">
-        <v>143</v>
+        <v>64</v>
       </c>
       <c r="C225" s="4" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="D225" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E225" s="5">
-        <v>0</v>
-      </c>
-      <c r="F225" s="5">
-        <v>10</v>
-      </c>
-      <c r="G225" s="5">
-        <v>0.1</v>
+        <v>63</v>
+      </c>
+      <c r="E225" s="5"/>
+      <c r="F225" s="5"/>
+      <c r="G225" s="5" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="226" spans="1:7" x14ac:dyDescent="0.25">
@@ -5908,30 +5912,26 @@
         <v>143</v>
       </c>
       <c r="C226" s="4" t="s">
-        <v>45</v>
+        <v>144</v>
       </c>
       <c r="D226" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E226" s="5">
-        <v>0</v>
-      </c>
-      <c r="F226" s="5">
-        <v>10</v>
-      </c>
-      <c r="G226" s="5">
-        <v>0.1</v>
+        <v>63</v>
+      </c>
+      <c r="E226" s="5"/>
+      <c r="F226" s="5"/>
+      <c r="G226" s="5" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="227" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A227" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="B227" s="4" t="s">
-        <v>145</v>
+      <c r="B227" s="2" t="s">
+        <v>143</v>
       </c>
       <c r="C227" s="4" t="s">
-        <v>146</v>
+        <v>44</v>
       </c>
       <c r="D227" s="5" t="s">
         <v>5</v>
@@ -5940,10 +5940,10 @@
         <v>0</v>
       </c>
       <c r="F227" s="5">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="G227" s="5">
-        <v>25</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="228" spans="1:7" x14ac:dyDescent="0.25">
@@ -5951,33 +5951,33 @@
         <v>214</v>
       </c>
       <c r="B228" s="2" t="s">
-        <v>211</v>
+        <v>143</v>
       </c>
       <c r="C228" s="4" t="s">
-        <v>147</v>
+        <v>45</v>
       </c>
       <c r="D228" s="5" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E228" s="5">
         <v>0</v>
       </c>
       <c r="F228" s="5">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G228" s="5">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="229" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A229" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="B229" s="2" t="s">
-        <v>211</v>
+      <c r="B229" s="4" t="s">
+        <v>145</v>
       </c>
       <c r="C229" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D229" s="5" t="s">
         <v>5</v>
@@ -5989,7 +5989,7 @@
         <v>100</v>
       </c>
       <c r="G229" s="5">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="230" spans="1:7" x14ac:dyDescent="0.25">
@@ -6000,19 +6000,19 @@
         <v>211</v>
       </c>
       <c r="C230" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D230" s="5" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="E230" s="5">
         <v>0</v>
       </c>
       <c r="F230" s="5">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G230" s="5">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="231" spans="1:7" x14ac:dyDescent="0.25">
@@ -6023,7 +6023,7 @@
         <v>211</v>
       </c>
       <c r="C231" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D231" s="5" t="s">
         <v>5</v>
@@ -6032,10 +6032,10 @@
         <v>0</v>
       </c>
       <c r="F231" s="5">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="G231" s="5">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="232" spans="1:7" x14ac:dyDescent="0.25">
@@ -6046,7 +6046,7 @@
         <v>211</v>
       </c>
       <c r="C232" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D232" s="5" t="s">
         <v>5</v>
@@ -6058,7 +6058,7 @@
         <v>10</v>
       </c>
       <c r="G232" s="5">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="233" spans="1:7" x14ac:dyDescent="0.25">
@@ -6069,7 +6069,7 @@
         <v>211</v>
       </c>
       <c r="C233" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D233" s="5" t="s">
         <v>5</v>
@@ -6081,7 +6081,7 @@
         <v>10</v>
       </c>
       <c r="G233" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.25">
@@ -6092,7 +6092,7 @@
         <v>211</v>
       </c>
       <c r="C234" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D234" s="5" t="s">
         <v>5</v>
@@ -6104,52 +6104,60 @@
         <v>10</v>
       </c>
       <c r="G234" s="5">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="235" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A235" s="2" t="s">
-        <v>228</v>
+        <v>214</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>228</v>
+        <v>211</v>
       </c>
       <c r="C235" s="4" t="s">
-        <v>220</v>
-      </c>
-      <c r="D235" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E235" s="7"/>
-      <c r="F235" s="7"/>
-      <c r="G235" s="12" t="s">
-        <v>238</v>
+        <v>152</v>
+      </c>
+      <c r="D235" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E235" s="5">
+        <v>0</v>
+      </c>
+      <c r="F235" s="5">
+        <v>10</v>
+      </c>
+      <c r="G235" s="5">
+        <v>0</v>
       </c>
     </row>
     <row r="236" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A236" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="B236" s="7" t="s">
-        <v>231</v>
+        <v>214</v>
+      </c>
+      <c r="B236" s="2" t="s">
+        <v>211</v>
       </c>
       <c r="C236" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="D236" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E236" s="7"/>
-      <c r="F236" s="7"/>
-      <c r="G236" s="6" t="s">
-        <v>233</v>
+        <v>153</v>
+      </c>
+      <c r="D236" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E236" s="5">
+        <v>0</v>
+      </c>
+      <c r="F236" s="5">
+        <v>10</v>
+      </c>
+      <c r="G236" s="5">
+        <v>0</v>
       </c>
     </row>
     <row r="237" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A237" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="B237" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="B237" s="2" t="s">
         <v>228</v>
       </c>
       <c r="C237" s="4" t="s">
@@ -6158,7 +6166,45 @@
       <c r="D237" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G237" t="s">
+      <c r="E237" s="7"/>
+      <c r="F237" s="7"/>
+      <c r="G237" s="12" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A238" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="B238" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C238" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="D238" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E238" s="7"/>
+      <c r="F238" s="7"/>
+      <c r="G238" s="6" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="239" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A239" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="B239" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="C239" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="D239" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G239" t="s">
         <v>234</v>
       </c>
     </row>

</xml_diff>